<commit_message>
reorganization genetic initialization code
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -652,187 +652,187 @@
               <c:numCache>
                 <c:ptCount val="61"/>
                 <c:pt idx="0">
-                  <c:v>0.2647430569296756</c:v>
+                  <c:v>0.25385405913030923</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2542345592423763</c:v>
+                  <c:v>0.23493005682721724</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.24347910478509804</c:v>
+                  <c:v>0.23620012671432528</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.24796615294023178</c:v>
+                  <c:v>0.27954658841439545</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.2796565310567929</c:v>
+                  <c:v>0.2537648004717664</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.27885143374197807</c:v>
+                  <c:v>0.24694905260139216</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.27429741675018326</c:v>
+                  <c:v>0.24403045852383065</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.2731926948741994</c:v>
+                  <c:v>0.24453365254631745</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.27326263061108935</c:v>
+                  <c:v>0.24666798958238953</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.26751543899893837</c:v>
+                  <c:v>0.24583811340227155</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.26017695810495434</c:v>
+                  <c:v>0.25179985559160456</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.28798428440484053</c:v>
+                  <c:v>0.27242573395598507</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.29254624968490056</c:v>
+                  <c:v>0.25602693100864793</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.2733906835106401</c:v>
+                  <c:v>0.2646881981053287</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.26696570855713336</c:v>
+                  <c:v>0.2489368314622166</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.2617361595612093</c:v>
+                  <c:v>0.24561692903668075</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.26119458835663073</c:v>
+                  <c:v>0.26116868065074955</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.2761340155906682</c:v>
+                  <c:v>0.2500092037952017</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.2583281399477745</c:v>
+                  <c:v>0.24614755975586275</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.2478327091846529</c:v>
+                  <c:v>0.23129864235600842</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.23829046215249844</c:v>
+                  <c:v>0.2321948147156281</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.240854886857952</c:v>
+                  <c:v>0.2394840352627732</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.25047783983929794</c:v>
+                  <c:v>0.23211265813536103</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.24883522878306188</c:v>
+                  <c:v>0.22104525806303954</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.24044656857291102</c:v>
+                  <c:v>0.20528601275261193</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.2193438069112776</c:v>
+                  <c:v>0.19613881844534028</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.21081796239651907</c:v>
+                  <c:v>0.19242049848292878</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.19925817781310928</c:v>
+                  <c:v>0.18899065532511425</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.20457373705359183</c:v>
+                  <c:v>0.19445511934915635</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.1978794269620103</c:v>
+                  <c:v>0.20080732820829467</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.20513883192467805</c:v>
+                  <c:v>0.1717461099846498</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.1825234342306371</c:v>
+                  <c:v>0.1593696224863909</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.1738256744313484</c:v>
+                  <c:v>0.1441111575314644</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.16315250771086498</c:v>
+                  <c:v>0.14634845049670148</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.16408659078813886</c:v>
+                  <c:v>0.16944285308808746</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.19145791054573552</c:v>
+                  <c:v>0.1841518431774174</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.1959809458414209</c:v>
+                  <c:v>0.17593322036020123</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.18889673476156665</c:v>
+                  <c:v>0.15409054491860893</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.17921567072335287</c:v>
+                  <c:v>0.17470571549463848</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.19085814796540182</c:v>
+                  <c:v>0.1731983141123689</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.19739051822679596</c:v>
+                  <c:v>0.16968407162092386</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.19348602785854</c:v>
+                  <c:v>0.1873128974756765</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.20521596788101737</c:v>
+                  <c:v>0.19751667771031614</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.2288860903474048</c:v>
+                  <c:v>0.20540850833403387</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.21854426202873187</c:v>
+                  <c:v>0.20945865620530651</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.21468958318605222</c:v>
+                  <c:v>0.22027734456284323</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.22297815985403877</c:v>
+                  <c:v>0.2160829303290156</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.2240970472181413</c:v>
+                  <c:v>0.21019801485231562</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.22199671118247893</c:v>
+                  <c:v>0.19735210741154838</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.20356581480892277</c:v>
+                  <c:v>0.21185634372326648</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.23246244294101784</c:v>
+                  <c:v>0.22786783984417752</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.2367375281887646</c:v>
+                  <c:v>0.21648475786800309</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.23057661686915493</c:v>
+                  <c:v>0.2419200744799142</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.24860799411284856</c:v>
+                  <c:v>0.236663641795989</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.2598960265559911</c:v>
+                  <c:v>0.2455847376168069</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.24760113402814748</c:v>
+                  <c:v>0.23444219756433507</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.26499253939249734</c:v>
+                  <c:v>0.22259836365105878</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.260895328188542</c:v>
+                  <c:v>0.2500403933274996</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.27183425869442623</c:v>
+                  <c:v>0.25190069002649057</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.2666331272446599</c:v>
+                  <c:v>0.25347578651007163</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.26644683881854686</c:v>
+                  <c:v>0.2641012279369823</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -934,7 +934,7 @@
         <v>0.24673684210526317</v>
       </c>
       <c r="C1" t="n">
-        <v>0.2647430569296756</v>
+        <v>0.25385405913030923</v>
       </c>
     </row>
     <row r="2">
@@ -945,7 +945,7 @@
         <v>0.22342105263157896</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2542345592423763</v>
+        <v>0.23493005682721724</v>
       </c>
     </row>
     <row r="3">
@@ -956,7 +956,7 @@
         <v>0.2627894736842105</v>
       </c>
       <c r="C3" t="n">
-        <v>0.24347910478509804</v>
+        <v>0.23620012671432528</v>
       </c>
     </row>
     <row r="4">
@@ -967,7 +967,7 @@
         <v>0.26563157894736844</v>
       </c>
       <c r="C4" t="n">
-        <v>0.24796615294023178</v>
+        <v>0.27954658841439545</v>
       </c>
     </row>
     <row r="5">
@@ -978,7 +978,7 @@
         <v>0.2513684210526316</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2796565310567929</v>
+        <v>0.2537648004717664</v>
       </c>
     </row>
     <row r="6">
@@ -989,7 +989,7 @@
         <v>0.2583157894736842</v>
       </c>
       <c r="C6" t="n">
-        <v>0.27885143374197807</v>
+        <v>0.24694905260139216</v>
       </c>
     </row>
     <row r="7">
@@ -1000,7 +1000,7 @@
         <v>0.26305263157894737</v>
       </c>
       <c r="C7" t="n">
-        <v>0.27429741675018326</v>
+        <v>0.24403045852383065</v>
       </c>
     </row>
     <row r="8">
@@ -1011,7 +1011,7 @@
         <v>0.2564736842105263</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2731926948741994</v>
+        <v>0.24453365254631745</v>
       </c>
     </row>
     <row r="9">
@@ -1022,7 +1022,7 @@
         <v>0.254421052631579</v>
       </c>
       <c r="C9" t="n">
-        <v>0.27326263061108935</v>
+        <v>0.24666798958238953</v>
       </c>
     </row>
     <row r="10">
@@ -1033,7 +1033,7 @@
         <v>0.25494736842105264</v>
       </c>
       <c r="C10" t="n">
-        <v>0.26751543899893837</v>
+        <v>0.24583811340227155</v>
       </c>
     </row>
     <row r="11">
@@ -1044,7 +1044,7 @@
         <v>0.25905263157894737</v>
       </c>
       <c r="C11" t="n">
-        <v>0.26017695810495434</v>
+        <v>0.25179985559160456</v>
       </c>
     </row>
     <row r="12">
@@ -1055,7 +1055,7 @@
         <v>0.2759473684210526</v>
       </c>
       <c r="C12" t="n">
-        <v>0.28798428440484053</v>
+        <v>0.27242573395598507</v>
       </c>
     </row>
     <row r="13">
@@ -1066,7 +1066,7 @@
         <v>0.26094736842105265</v>
       </c>
       <c r="C13" t="n">
-        <v>0.29254624968490056</v>
+        <v>0.25602693100864793</v>
       </c>
     </row>
     <row r="14">
@@ -1077,7 +1077,7 @@
         <v>0.25742105263157894</v>
       </c>
       <c r="C14" t="n">
-        <v>0.2733906835106401</v>
+        <v>0.2646881981053287</v>
       </c>
     </row>
     <row r="15">
@@ -1088,7 +1088,7 @@
         <v>0.25305263157894736</v>
       </c>
       <c r="C15" t="n">
-        <v>0.26696570855713336</v>
+        <v>0.2489368314622166</v>
       </c>
     </row>
     <row r="16">
@@ -1099,7 +1099,7 @@
         <v>0.25852631578947366</v>
       </c>
       <c r="C16" t="n">
-        <v>0.2617361595612093</v>
+        <v>0.24561692903668075</v>
       </c>
     </row>
     <row r="17">
@@ -1110,7 +1110,7 @@
         <v>0.2566842105263158</v>
       </c>
       <c r="C17" t="n">
-        <v>0.26119458835663073</v>
+        <v>0.26116868065074955</v>
       </c>
     </row>
     <row r="18">
@@ -1121,7 +1121,7 @@
         <v>0.25084210526315787</v>
       </c>
       <c r="C18" t="n">
-        <v>0.2761340155906682</v>
+        <v>0.2500092037952017</v>
       </c>
     </row>
     <row r="19">
@@ -1132,7 +1132,7 @@
         <v>0.2452105263157895</v>
       </c>
       <c r="C19" t="n">
-        <v>0.2583281399477745</v>
+        <v>0.24614755975586275</v>
       </c>
     </row>
     <row r="20">
@@ -1143,7 +1143,7 @@
         <v>0.23610526315789473</v>
       </c>
       <c r="C20" t="n">
-        <v>0.2478327091846529</v>
+        <v>0.23129864235600842</v>
       </c>
     </row>
     <row r="21">
@@ -1154,7 +1154,7 @@
         <v>0.23410526315789473</v>
       </c>
       <c r="C21" t="n">
-        <v>0.23829046215249844</v>
+        <v>0.2321948147156281</v>
       </c>
     </row>
     <row r="22">
@@ -1165,7 +1165,7 @@
         <v>0.24357894736842106</v>
       </c>
       <c r="C22" t="n">
-        <v>0.240854886857952</v>
+        <v>0.2394840352627732</v>
       </c>
     </row>
     <row r="23">
@@ -1176,7 +1176,7 @@
         <v>0.23421052631578948</v>
       </c>
       <c r="C23" t="n">
-        <v>0.25047783983929794</v>
+        <v>0.23211265813536103</v>
       </c>
     </row>
     <row r="24">
@@ -1187,7 +1187,7 @@
         <v>0.2274736842105263</v>
       </c>
       <c r="C24" t="n">
-        <v>0.24883522878306188</v>
+        <v>0.22104525806303954</v>
       </c>
     </row>
     <row r="25">
@@ -1198,7 +1198,7 @@
         <v>0.21226315789473682</v>
       </c>
       <c r="C25" t="n">
-        <v>0.24044656857291102</v>
+        <v>0.20528601275261193</v>
       </c>
     </row>
     <row r="26">
@@ -1209,7 +1209,7 @@
         <v>0.19994736842105265</v>
       </c>
       <c r="C26" t="n">
-        <v>0.2193438069112776</v>
+        <v>0.19613881844534028</v>
       </c>
     </row>
     <row r="27">
@@ -1220,7 +1220,7 @@
         <v>0.19236842105263158</v>
       </c>
       <c r="C27" t="n">
-        <v>0.21081796239651907</v>
+        <v>0.19242049848292878</v>
       </c>
     </row>
     <row r="28">
@@ -1231,7 +1231,7 @@
         <v>0.19889473684210526</v>
       </c>
       <c r="C28" t="n">
-        <v>0.19925817781310928</v>
+        <v>0.18899065532511425</v>
       </c>
     </row>
     <row r="29">
@@ -1242,7 +1242,7 @@
         <v>0.19678947368421054</v>
       </c>
       <c r="C29" t="n">
-        <v>0.20457373705359183</v>
+        <v>0.19445511934915635</v>
       </c>
     </row>
     <row r="30">
@@ -1253,7 +1253,7 @@
         <v>0.1964736842105263</v>
       </c>
       <c r="C30" t="n">
-        <v>0.1978794269620103</v>
+        <v>0.20080732820829467</v>
       </c>
     </row>
     <row r="31">
@@ -1264,7 +1264,7 @@
         <v>0.17505263157894735</v>
       </c>
       <c r="C31" t="n">
-        <v>0.20513883192467805</v>
+        <v>0.1717461099846498</v>
       </c>
     </row>
     <row r="32">
@@ -1275,7 +1275,7 @@
         <v>0.1591578947368421</v>
       </c>
       <c r="C32" t="n">
-        <v>0.1825234342306371</v>
+        <v>0.1593696224863909</v>
       </c>
     </row>
     <row r="33">
@@ -1286,7 +1286,7 @@
         <v>0.15126315789473682</v>
       </c>
       <c r="C33" t="n">
-        <v>0.1738256744313484</v>
+        <v>0.1441111575314644</v>
       </c>
     </row>
     <row r="34">
@@ -1297,7 +1297,7 @@
         <v>0.16884210526315788</v>
       </c>
       <c r="C34" t="n">
-        <v>0.16315250771086498</v>
+        <v>0.14634845049670148</v>
       </c>
     </row>
     <row r="35">
@@ -1308,7 +1308,7 @@
         <v>0.1818421052631579</v>
       </c>
       <c r="C35" t="n">
-        <v>0.16408659078813886</v>
+        <v>0.16944285308808746</v>
       </c>
     </row>
     <row r="36">
@@ -1319,7 +1319,7 @@
         <v>0.17142105263157895</v>
       </c>
       <c r="C36" t="n">
-        <v>0.19145791054573552</v>
+        <v>0.1841518431774174</v>
       </c>
     </row>
     <row r="37">
@@ -1330,7 +1330,7 @@
         <v>0.17831578947368423</v>
       </c>
       <c r="C37" t="n">
-        <v>0.1959809458414209</v>
+        <v>0.17593322036020123</v>
       </c>
     </row>
     <row r="38">
@@ -1341,7 +1341,7 @@
         <v>0.1638421052631579</v>
       </c>
       <c r="C38" t="n">
-        <v>0.18889673476156665</v>
+        <v>0.15409054491860893</v>
       </c>
     </row>
     <row r="39">
@@ -1352,7 +1352,7 @@
         <v>0.16999999999999998</v>
       </c>
       <c r="C39" t="n">
-        <v>0.17921567072335287</v>
+        <v>0.17470571549463848</v>
       </c>
     </row>
     <row r="40">
@@ -1363,7 +1363,7 @@
         <v>0.17352631578947367</v>
       </c>
       <c r="C40" t="n">
-        <v>0.19085814796540182</v>
+        <v>0.1731983141123689</v>
       </c>
     </row>
     <row r="41">
@@ -1374,7 +1374,7 @@
         <v>0.1845263157894737</v>
       </c>
       <c r="C41" t="n">
-        <v>0.19739051822679596</v>
+        <v>0.16968407162092386</v>
       </c>
     </row>
     <row r="42">
@@ -1385,7 +1385,7 @@
         <v>0.19263157894736843</v>
       </c>
       <c r="C42" t="n">
-        <v>0.19348602785854</v>
+        <v>0.1873128974756765</v>
       </c>
     </row>
     <row r="43">
@@ -1396,7 +1396,7 @@
         <v>0.2053157894736842</v>
       </c>
       <c r="C43" t="n">
-        <v>0.20521596788101737</v>
+        <v>0.19751667771031614</v>
       </c>
     </row>
     <row r="44">
@@ -1407,7 +1407,7 @@
         <v>0.21136842105263157</v>
       </c>
       <c r="C44" t="n">
-        <v>0.2288860903474048</v>
+        <v>0.20540850833403387</v>
       </c>
     </row>
     <row r="45">
@@ -1418,7 +1418,7 @@
         <v>0.20500000000000002</v>
       </c>
       <c r="C45" t="n">
-        <v>0.21854426202873187</v>
+        <v>0.20945865620530651</v>
       </c>
     </row>
     <row r="46">
@@ -1429,7 +1429,7 @@
         <v>0.21610526315789474</v>
       </c>
       <c r="C46" t="n">
-        <v>0.21468958318605222</v>
+        <v>0.22027734456284323</v>
       </c>
     </row>
     <row r="47">
@@ -1440,7 +1440,7 @@
         <v>0.21289473684210528</v>
       </c>
       <c r="C47" t="n">
-        <v>0.22297815985403877</v>
+        <v>0.2160829303290156</v>
       </c>
     </row>
     <row r="48">
@@ -1451,7 +1451,7 @@
         <v>0.21021052631578946</v>
       </c>
       <c r="C48" t="n">
-        <v>0.2240970472181413</v>
+        <v>0.21019801485231562</v>
       </c>
     </row>
     <row r="49">
@@ -1462,7 +1462,7 @@
         <v>0.19778947368421052</v>
       </c>
       <c r="C49" t="n">
-        <v>0.22199671118247893</v>
+        <v>0.19735210741154838</v>
       </c>
     </row>
     <row r="50">
@@ -1473,7 +1473,7 @@
         <v>0.22047368421052632</v>
       </c>
       <c r="C50" t="n">
-        <v>0.20356581480892277</v>
+        <v>0.21185634372326648</v>
       </c>
     </row>
     <row r="51">
@@ -1484,7 +1484,7 @@
         <v>0.23105263157894737</v>
       </c>
       <c r="C51" t="n">
-        <v>0.23246244294101784</v>
+        <v>0.22786783984417752</v>
       </c>
     </row>
     <row r="52">
@@ -1495,7 +1495,7 @@
         <v>0.2271578947368421</v>
       </c>
       <c r="C52" t="n">
-        <v>0.2367375281887646</v>
+        <v>0.21648475786800309</v>
       </c>
     </row>
     <row r="53">
@@ -1506,7 +1506,7 @@
         <v>0.23768421052631578</v>
       </c>
       <c r="C53" t="n">
-        <v>0.23057661686915493</v>
+        <v>0.2419200744799142</v>
       </c>
     </row>
     <row r="54">
@@ -1517,7 +1517,7 @@
         <v>0.24736842105263157</v>
       </c>
       <c r="C54" t="n">
-        <v>0.24860799411284856</v>
+        <v>0.236663641795989</v>
       </c>
     </row>
     <row r="55">
@@ -1528,7 +1528,7 @@
         <v>0.2416315789473684</v>
       </c>
       <c r="C55" t="n">
-        <v>0.2598960265559911</v>
+        <v>0.2455847376168069</v>
       </c>
     </row>
     <row r="56">
@@ -1539,7 +1539,7 @@
         <v>0.2383157894736842</v>
       </c>
       <c r="C56" t="n">
-        <v>0.24760113402814748</v>
+        <v>0.23444219756433507</v>
       </c>
     </row>
     <row r="57">
@@ -1550,7 +1550,7 @@
         <v>0.24947368421052632</v>
       </c>
       <c r="C57" t="n">
-        <v>0.26499253939249734</v>
+        <v>0.22259836365105878</v>
       </c>
     </row>
     <row r="58">
@@ -1561,7 +1561,7 @@
         <v>0.2585789473684211</v>
       </c>
       <c r="C58" t="n">
-        <v>0.260895328188542</v>
+        <v>0.2500403933274996</v>
       </c>
     </row>
     <row r="59">
@@ -1572,7 +1572,7 @@
         <v>0.2565263157894737</v>
       </c>
       <c r="C59" t="n">
-        <v>0.27183425869442623</v>
+        <v>0.25190069002649057</v>
       </c>
     </row>
     <row r="60">
@@ -1583,7 +1583,7 @@
         <v>0.262</v>
       </c>
       <c r="C60" t="n">
-        <v>0.2666331272446599</v>
+        <v>0.25347578651007163</v>
       </c>
     </row>
     <row r="61">
@@ -1594,7 +1594,7 @@
         <v>0.26063157894736844</v>
       </c>
       <c r="C61" t="n">
-        <v>0.26644683881854686</v>
+        <v>0.2641012279369823</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix some bags annealing
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -652,187 +652,187 @@
               <c:numCache>
                 <c:ptCount val="61"/>
                 <c:pt idx="0">
-                  <c:v>0.26576278731553055</c:v>
+                  <c:v>0.267401418239127</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2529275347502502</c:v>
+                  <c:v>0.24897750791962808</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25294371658276515</c:v>
+                  <c:v>0.2627901331252257</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.24910794104260886</c:v>
+                  <c:v>0.26772838101863683</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.2772648242406388</c:v>
+                  <c:v>0.2702240058091856</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.2797659378535549</c:v>
+                  <c:v>0.2730778968229175</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.27218631203632776</c:v>
+                  <c:v>0.2635058189048585</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.26948314018403574</c:v>
+                  <c:v>0.2600769108469877</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.27162540363621174</c:v>
+                  <c:v>0.2648143882721631</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.2669925656000222</c:v>
+                  <c:v>0.2630063011413475</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.26083639362847344</c:v>
+                  <c:v>0.2630977588567175</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.29133794183374295</c:v>
+                  <c:v>0.2935191727858457</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.28559745205023074</c:v>
+                  <c:v>0.27063860951765567</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.27512721481818575</c:v>
+                  <c:v>0.2784289987799062</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.2668532325028858</c:v>
+                  <c:v>0.26468244181050865</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.26038526254789096</c:v>
+                  <c:v>0.25783551158516377</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.2643415532975203</c:v>
+                  <c:v>0.27211596312316044</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.27180359118038006</c:v>
+                  <c:v>0.26295521687123025</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.25825283457145604</c:v>
+                  <c:v>0.2583138744156222</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.24714317280682307</c:v>
+                  <c:v>0.2447138787297614</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.2399128418443566</c:v>
+                  <c:v>0.243486482945483</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.24536319863853767</c:v>
+                  <c:v>0.25334877452007404</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.24923826829051463</c:v>
+                  <c:v>0.2456524353884703</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.24841363677444883</c:v>
+                  <c:v>0.2416707670640687</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.23478992668463058</c:v>
+                  <c:v>0.22045691010866228</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.21667944724953508</c:v>
+                  <c:v>0.2093145951327903</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.20785963456455306</c:v>
+                  <c:v>0.20202630075524836</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.19972558829572248</c:v>
+                  <c:v>0.19986494199941948</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.20234619399593926</c:v>
+                  <c:v>0.20036454885809873</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.20272272750830925</c:v>
+                  <c:v>0.21189229315365393</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.19856782333885745</c:v>
+                  <c:v>0.18348404832268672</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.17774823129236947</c:v>
+                  <c:v>0.16789280290606534</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.16693117633183818</c:v>
+                  <c:v>0.15244998401603155</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.16540314403410217</c:v>
+                  <c:v>0.16369919724812765</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.17158958346879874</c:v>
+                  <c:v>0.18333665275997935</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.188403184673977</c:v>
+                  <c:v>0.18660267705914643</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.19320758968875035</c:v>
+                  <c:v>0.18657188148895543</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.18342479881279627</c:v>
+                  <c:v>0.16838226737650566</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.18299107998969102</c:v>
+                  <c:v>0.1878759266823054</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.1872818332048993</c:v>
+                  <c:v>0.1808323140185807</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.19659921548429554</c:v>
+                  <c:v>0.18856898432394953</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.19754312898462253</c:v>
+                  <c:v>0.20227253130958744</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.2100458124221859</c:v>
+                  <c:v>0.21504195806552795</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.2290586811692015</c:v>
+                  <c:v>0.22417616128791434</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.21791847624489125</c:v>
+                  <c:v>0.21798737841403187</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.21886532587742794</c:v>
+                  <c:v>0.2288757078376571</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.22241711735408418</c:v>
+                  <c:v>0.22351522638940718</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.2221440003302506</c:v>
+                  <c:v>0.21924587969978382</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.21802063621012926</c:v>
+                  <c:v>0.2090120769316686</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.20798256940091567</c:v>
+                  <c:v>0.21907450792844438</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.23752814514329826</c:v>
+                  <c:v>0.24451589273382995</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.23014912508230415</c:v>
+                  <c:v>0.22099331873925576</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.23442325185018423</c:v>
+                  <c:v>0.24679769905945964</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.2525440545645999</c:v>
+                  <c:v>0.2559122385310133</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.25920694689965523</c:v>
+                  <c:v>0.25791491026055147</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.2483296473356042</c:v>
+                  <c:v>0.24846585784938113</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.26261647845265995</c:v>
+                  <c:v>0.24861556803718318</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.2618518658227811</c:v>
+                  <c:v>0.2633753401200111</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.27135406690944003</c:v>
+                  <c:v>0.2681950936015137</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.26835679316009187</c:v>
+                  <c:v>0.26971037434614775</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.2698804217228156</c:v>
+                  <c:v>0.2770609242742207</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -934,7 +934,7 @@
         <v>0.24673684210526317</v>
       </c>
       <c r="C1" t="n">
-        <v>0.26576278731553055</v>
+        <v>0.267401418239127</v>
       </c>
     </row>
     <row r="2">
@@ -945,7 +945,7 @@
         <v>0.22342105263157896</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2529275347502502</v>
+        <v>0.24897750791962808</v>
       </c>
     </row>
     <row r="3">
@@ -956,7 +956,7 @@
         <v>0.2627894736842105</v>
       </c>
       <c r="C3" t="n">
-        <v>0.25294371658276515</v>
+        <v>0.2627901331252257</v>
       </c>
     </row>
     <row r="4">
@@ -967,7 +967,7 @@
         <v>0.26563157894736844</v>
       </c>
       <c r="C4" t="n">
-        <v>0.24910794104260886</v>
+        <v>0.26772838101863683</v>
       </c>
     </row>
     <row r="5">
@@ -978,7 +978,7 @@
         <v>0.2513684210526316</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2772648242406388</v>
+        <v>0.2702240058091856</v>
       </c>
     </row>
     <row r="6">
@@ -989,7 +989,7 @@
         <v>0.2583157894736842</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2797659378535549</v>
+        <v>0.2730778968229175</v>
       </c>
     </row>
     <row r="7">
@@ -1000,7 +1000,7 @@
         <v>0.26305263157894737</v>
       </c>
       <c r="C7" t="n">
-        <v>0.27218631203632776</v>
+        <v>0.2635058189048585</v>
       </c>
     </row>
     <row r="8">
@@ -1011,7 +1011,7 @@
         <v>0.2564736842105263</v>
       </c>
       <c r="C8" t="n">
-        <v>0.26948314018403574</v>
+        <v>0.2600769108469877</v>
       </c>
     </row>
     <row r="9">
@@ -1022,7 +1022,7 @@
         <v>0.254421052631579</v>
       </c>
       <c r="C9" t="n">
-        <v>0.27162540363621174</v>
+        <v>0.2648143882721631</v>
       </c>
     </row>
     <row r="10">
@@ -1033,7 +1033,7 @@
         <v>0.25494736842105264</v>
       </c>
       <c r="C10" t="n">
-        <v>0.2669925656000222</v>
+        <v>0.2630063011413475</v>
       </c>
     </row>
     <row r="11">
@@ -1044,7 +1044,7 @@
         <v>0.25905263157894737</v>
       </c>
       <c r="C11" t="n">
-        <v>0.26083639362847344</v>
+        <v>0.2630977588567175</v>
       </c>
     </row>
     <row r="12">
@@ -1055,7 +1055,7 @@
         <v>0.2759473684210526</v>
       </c>
       <c r="C12" t="n">
-        <v>0.29133794183374295</v>
+        <v>0.2935191727858457</v>
       </c>
     </row>
     <row r="13">
@@ -1066,7 +1066,7 @@
         <v>0.26094736842105265</v>
       </c>
       <c r="C13" t="n">
-        <v>0.28559745205023074</v>
+        <v>0.27063860951765567</v>
       </c>
     </row>
     <row r="14">
@@ -1077,7 +1077,7 @@
         <v>0.25742105263157894</v>
       </c>
       <c r="C14" t="n">
-        <v>0.27512721481818575</v>
+        <v>0.2784289987799062</v>
       </c>
     </row>
     <row r="15">
@@ -1088,7 +1088,7 @@
         <v>0.25305263157894736</v>
       </c>
       <c r="C15" t="n">
-        <v>0.2668532325028858</v>
+        <v>0.26468244181050865</v>
       </c>
     </row>
     <row r="16">
@@ -1099,7 +1099,7 @@
         <v>0.25852631578947366</v>
       </c>
       <c r="C16" t="n">
-        <v>0.26038526254789096</v>
+        <v>0.25783551158516377</v>
       </c>
     </row>
     <row r="17">
@@ -1110,7 +1110,7 @@
         <v>0.2566842105263158</v>
       </c>
       <c r="C17" t="n">
-        <v>0.2643415532975203</v>
+        <v>0.27211596312316044</v>
       </c>
     </row>
     <row r="18">
@@ -1121,7 +1121,7 @@
         <v>0.25084210526315787</v>
       </c>
       <c r="C18" t="n">
-        <v>0.27180359118038006</v>
+        <v>0.26295521687123025</v>
       </c>
     </row>
     <row r="19">
@@ -1132,7 +1132,7 @@
         <v>0.2452105263157895</v>
       </c>
       <c r="C19" t="n">
-        <v>0.25825283457145604</v>
+        <v>0.2583138744156222</v>
       </c>
     </row>
     <row r="20">
@@ -1143,7 +1143,7 @@
         <v>0.23610526315789473</v>
       </c>
       <c r="C20" t="n">
-        <v>0.24714317280682307</v>
+        <v>0.2447138787297614</v>
       </c>
     </row>
     <row r="21">
@@ -1154,7 +1154,7 @@
         <v>0.23410526315789473</v>
       </c>
       <c r="C21" t="n">
-        <v>0.2399128418443566</v>
+        <v>0.243486482945483</v>
       </c>
     </row>
     <row r="22">
@@ -1165,7 +1165,7 @@
         <v>0.24357894736842106</v>
       </c>
       <c r="C22" t="n">
-        <v>0.24536319863853767</v>
+        <v>0.25334877452007404</v>
       </c>
     </row>
     <row r="23">
@@ -1176,7 +1176,7 @@
         <v>0.23421052631578948</v>
       </c>
       <c r="C23" t="n">
-        <v>0.24923826829051463</v>
+        <v>0.2456524353884703</v>
       </c>
     </row>
     <row r="24">
@@ -1187,7 +1187,7 @@
         <v>0.2274736842105263</v>
       </c>
       <c r="C24" t="n">
-        <v>0.24841363677444883</v>
+        <v>0.2416707670640687</v>
       </c>
     </row>
     <row r="25">
@@ -1198,7 +1198,7 @@
         <v>0.21226315789473682</v>
       </c>
       <c r="C25" t="n">
-        <v>0.23478992668463058</v>
+        <v>0.22045691010866228</v>
       </c>
     </row>
     <row r="26">
@@ -1209,7 +1209,7 @@
         <v>0.19994736842105265</v>
       </c>
       <c r="C26" t="n">
-        <v>0.21667944724953508</v>
+        <v>0.2093145951327903</v>
       </c>
     </row>
     <row r="27">
@@ -1220,7 +1220,7 @@
         <v>0.19236842105263158</v>
       </c>
       <c r="C27" t="n">
-        <v>0.20785963456455306</v>
+        <v>0.20202630075524836</v>
       </c>
     </row>
     <row r="28">
@@ -1231,7 +1231,7 @@
         <v>0.19889473684210526</v>
       </c>
       <c r="C28" t="n">
-        <v>0.19972558829572248</v>
+        <v>0.19986494199941948</v>
       </c>
     </row>
     <row r="29">
@@ -1242,7 +1242,7 @@
         <v>0.19678947368421054</v>
       </c>
       <c r="C29" t="n">
-        <v>0.20234619399593926</v>
+        <v>0.20036454885809873</v>
       </c>
     </row>
     <row r="30">
@@ -1253,7 +1253,7 @@
         <v>0.1964736842105263</v>
       </c>
       <c r="C30" t="n">
-        <v>0.20272272750830925</v>
+        <v>0.21189229315365393</v>
       </c>
     </row>
     <row r="31">
@@ -1264,7 +1264,7 @@
         <v>0.17505263157894735</v>
       </c>
       <c r="C31" t="n">
-        <v>0.19856782333885745</v>
+        <v>0.18348404832268672</v>
       </c>
     </row>
     <row r="32">
@@ -1275,7 +1275,7 @@
         <v>0.1591578947368421</v>
       </c>
       <c r="C32" t="n">
-        <v>0.17774823129236947</v>
+        <v>0.16789280290606534</v>
       </c>
     </row>
     <row r="33">
@@ -1286,7 +1286,7 @@
         <v>0.15126315789473682</v>
       </c>
       <c r="C33" t="n">
-        <v>0.16693117633183818</v>
+        <v>0.15244998401603155</v>
       </c>
     </row>
     <row r="34">
@@ -1297,7 +1297,7 @@
         <v>0.16884210526315788</v>
       </c>
       <c r="C34" t="n">
-        <v>0.16540314403410217</v>
+        <v>0.16369919724812765</v>
       </c>
     </row>
     <row r="35">
@@ -1308,7 +1308,7 @@
         <v>0.1818421052631579</v>
       </c>
       <c r="C35" t="n">
-        <v>0.17158958346879874</v>
+        <v>0.18333665275997935</v>
       </c>
     </row>
     <row r="36">
@@ -1319,7 +1319,7 @@
         <v>0.17142105263157895</v>
       </c>
       <c r="C36" t="n">
-        <v>0.188403184673977</v>
+        <v>0.18660267705914643</v>
       </c>
     </row>
     <row r="37">
@@ -1330,7 +1330,7 @@
         <v>0.17831578947368423</v>
       </c>
       <c r="C37" t="n">
-        <v>0.19320758968875035</v>
+        <v>0.18657188148895543</v>
       </c>
     </row>
     <row r="38">
@@ -1341,7 +1341,7 @@
         <v>0.1638421052631579</v>
       </c>
       <c r="C38" t="n">
-        <v>0.18342479881279627</v>
+        <v>0.16838226737650566</v>
       </c>
     </row>
     <row r="39">
@@ -1352,7 +1352,7 @@
         <v>0.16999999999999998</v>
       </c>
       <c r="C39" t="n">
-        <v>0.18299107998969102</v>
+        <v>0.1878759266823054</v>
       </c>
     </row>
     <row r="40">
@@ -1363,7 +1363,7 @@
         <v>0.17352631578947367</v>
       </c>
       <c r="C40" t="n">
-        <v>0.1872818332048993</v>
+        <v>0.1808323140185807</v>
       </c>
     </row>
     <row r="41">
@@ -1374,7 +1374,7 @@
         <v>0.1845263157894737</v>
       </c>
       <c r="C41" t="n">
-        <v>0.19659921548429554</v>
+        <v>0.18856898432394953</v>
       </c>
     </row>
     <row r="42">
@@ -1385,7 +1385,7 @@
         <v>0.19263157894736843</v>
       </c>
       <c r="C42" t="n">
-        <v>0.19754312898462253</v>
+        <v>0.20227253130958744</v>
       </c>
     </row>
     <row r="43">
@@ -1396,7 +1396,7 @@
         <v>0.2053157894736842</v>
       </c>
       <c r="C43" t="n">
-        <v>0.2100458124221859</v>
+        <v>0.21504195806552795</v>
       </c>
     </row>
     <row r="44">
@@ -1407,7 +1407,7 @@
         <v>0.21136842105263157</v>
       </c>
       <c r="C44" t="n">
-        <v>0.2290586811692015</v>
+        <v>0.22417616128791434</v>
       </c>
     </row>
     <row r="45">
@@ -1418,7 +1418,7 @@
         <v>0.20500000000000002</v>
       </c>
       <c r="C45" t="n">
-        <v>0.21791847624489125</v>
+        <v>0.21798737841403187</v>
       </c>
     </row>
     <row r="46">
@@ -1429,7 +1429,7 @@
         <v>0.21610526315789474</v>
       </c>
       <c r="C46" t="n">
-        <v>0.21886532587742794</v>
+        <v>0.2288757078376571</v>
       </c>
     </row>
     <row r="47">
@@ -1440,7 +1440,7 @@
         <v>0.21289473684210528</v>
       </c>
       <c r="C47" t="n">
-        <v>0.22241711735408418</v>
+        <v>0.22351522638940718</v>
       </c>
     </row>
     <row r="48">
@@ -1451,7 +1451,7 @@
         <v>0.21021052631578946</v>
       </c>
       <c r="C48" t="n">
-        <v>0.2221440003302506</v>
+        <v>0.21924587969978382</v>
       </c>
     </row>
     <row r="49">
@@ -1462,7 +1462,7 @@
         <v>0.19778947368421052</v>
       </c>
       <c r="C49" t="n">
-        <v>0.21802063621012926</v>
+        <v>0.2090120769316686</v>
       </c>
     </row>
     <row r="50">
@@ -1473,7 +1473,7 @@
         <v>0.22047368421052632</v>
       </c>
       <c r="C50" t="n">
-        <v>0.20798256940091567</v>
+        <v>0.21907450792844438</v>
       </c>
     </row>
     <row r="51">
@@ -1484,7 +1484,7 @@
         <v>0.23105263157894737</v>
       </c>
       <c r="C51" t="n">
-        <v>0.23752814514329826</v>
+        <v>0.24451589273382995</v>
       </c>
     </row>
     <row r="52">
@@ -1495,7 +1495,7 @@
         <v>0.2271578947368421</v>
       </c>
       <c r="C52" t="n">
-        <v>0.23014912508230415</v>
+        <v>0.22099331873925576</v>
       </c>
     </row>
     <row r="53">
@@ -1506,7 +1506,7 @@
         <v>0.23768421052631578</v>
       </c>
       <c r="C53" t="n">
-        <v>0.23442325185018423</v>
+        <v>0.24679769905945964</v>
       </c>
     </row>
     <row r="54">
@@ -1517,7 +1517,7 @@
         <v>0.24736842105263157</v>
       </c>
       <c r="C54" t="n">
-        <v>0.2525440545645999</v>
+        <v>0.2559122385310133</v>
       </c>
     </row>
     <row r="55">
@@ -1528,7 +1528,7 @@
         <v>0.2416315789473684</v>
       </c>
       <c r="C55" t="n">
-        <v>0.25920694689965523</v>
+        <v>0.25791491026055147</v>
       </c>
     </row>
     <row r="56">
@@ -1539,7 +1539,7 @@
         <v>0.2383157894736842</v>
       </c>
       <c r="C56" t="n">
-        <v>0.2483296473356042</v>
+        <v>0.24846585784938113</v>
       </c>
     </row>
     <row r="57">
@@ -1550,7 +1550,7 @@
         <v>0.24947368421052632</v>
       </c>
       <c r="C57" t="n">
-        <v>0.26261647845265995</v>
+        <v>0.24861556803718318</v>
       </c>
     </row>
     <row r="58">
@@ -1561,7 +1561,7 @@
         <v>0.2585789473684211</v>
       </c>
       <c r="C58" t="n">
-        <v>0.2618518658227811</v>
+        <v>0.2633753401200111</v>
       </c>
     </row>
     <row r="59">
@@ -1572,7 +1572,7 @@
         <v>0.2565263157894737</v>
       </c>
       <c r="C59" t="n">
-        <v>0.27135406690944003</v>
+        <v>0.2681950936015137</v>
       </c>
     </row>
     <row r="60">
@@ -1583,7 +1583,7 @@
         <v>0.262</v>
       </c>
       <c r="C60" t="n">
-        <v>0.26835679316009187</v>
+        <v>0.26971037434614775</v>
       </c>
     </row>
     <row r="61">
@@ -1594,7 +1594,7 @@
         <v>0.26063157894736844</v>
       </c>
       <c r="C61" t="n">
-        <v>0.2698804217228156</v>
+        <v>0.2770609242742207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>